<commit_message>
g3.9 - remoção de ano no nome da aba para evitar futuros erros
</commit_message>
<xml_diff>
--- a/Data/g3.9a.xlsx
+++ b/Data/g3.9a.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.11a 2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.11a" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Posição</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ano</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>2</v>
       </c>
+      <c r="D3" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>3</v>
       </c>
+      <c r="D4" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>4</v>
       </c>
+      <c r="D5" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>5</v>
       </c>
+      <c r="D6" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>6</v>
       </c>
+      <c r="D7" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -538,6 +561,9 @@
         <v>12.47469002329323</v>
       </c>
       <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -549,6 +575,9 @@
         <v>16.0557975886993</v>
       </c>
       <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>2023</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>